<commit_message>
Forgot about a point, fixed the animation and its table
</commit_message>
<xml_diff>
--- a/animazione/Notizie/Tabelle calcoli/19-01-2019.xlsx
+++ b/animazione/Notizie/Tabelle calcoli/19-01-2019.xlsx
@@ -13,7 +13,8 @@
     <sheet name="Foglio4" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_19_01_2019" localSheetId="3">Foglio4!$A$1:$H$117</definedName>
+    <definedName name="_19_01_2019" localSheetId="3">Foglio4!#REF!</definedName>
+    <definedName name="_19_01_2019_1" localSheetId="3">Foglio4!$A$1:$H$117</definedName>
     <definedName name="lunghezza" localSheetId="2">Foglio3!$G$1:$G$117</definedName>
     <definedName name="punti_animazione_semplificato" localSheetId="2">Foglio3!$A$1:$F$117</definedName>
   </definedNames>
@@ -37,7 +38,21 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="lunghezza" type="6" refreshedVersion="4" background="1" saveData="1">
+  <connection id="2" name="19-01-20191" type="6" refreshedVersion="4" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\Users\WORK\Desktop\Progetto Territoriale\Il-Binario-20-Bis\animazione\Notizie\19-01-2019.csv" decimal="," thousands="." semicolon="1">
+      <textFields count="8">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="lunghezza" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\WORK\Desktop\Progetto Territoriale\Il-Binario-20-Bis\animazione\lunghezza.csv" thousands=" " comma="1">
       <textFields count="7">
         <textField type="skip"/>
@@ -50,7 +65,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="punti animazione semplificato" type="6" refreshedVersion="4" background="1" saveData="1">
+  <connection id="4" name="punti animazione semplificato" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\WORK\Desktop\Progetto Territoriale\Il-Binario-20-Bis\animazione\punti animazione semplificato.csv" decimal="," thousands="." semicolon="1">
       <textFields count="6">
         <textField/>
@@ -204,7 +219,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="dd\-mm\-yyyy\ hh:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="dd\-mm\-yyyy\ hh:mm:ss"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -297,8 +312,8 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -319,15 +334,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="punti animazione semplificato" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="punti animazione semplificato" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="lunghezza" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="lunghezza" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="19-01-2019" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="19-01-2019_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -705,21 +720,21 @@
         <v>12</v>
       </c>
       <c r="B3" s="2">
-        <f>H2 + TIME(0,1,0)</f>
+        <f t="shared" ref="B3:B8" si="0">H2 + TIME(0,1,0)</f>
         <v>0.54930555555555549</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3" s="10">
-        <f>B3+TIME(0,C3,0)</f>
+        <f t="shared" ref="D3:D8" si="1">B3+TIME(0,C3,0)</f>
         <v>0.54930555555555549</v>
       </c>
       <c r="E3" s="12">
         <v>15</v>
       </c>
       <c r="F3" s="2">
-        <f>D3+TIME(0,E3,0)</f>
+        <f t="shared" ref="F3:F8" si="2">D3+TIME(0,E3,0)</f>
         <v>0.55972222222222212</v>
       </c>
       <c r="G3" s="6">
@@ -741,21 +756,21 @@
         <v>11</v>
       </c>
       <c r="B4" s="2">
-        <f>H3 + TIME(0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0.56041666666666656</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4" s="10">
-        <f>B4+TIME(0,C4,0)</f>
+        <f t="shared" si="1"/>
         <v>0.56041666666666656</v>
       </c>
       <c r="E4" s="12">
         <v>15</v>
       </c>
       <c r="F4" s="2">
-        <f>D4+TIME(0,E4,0)</f>
+        <f t="shared" si="2"/>
         <v>0.57083333333333319</v>
       </c>
       <c r="G4" s="6">
@@ -777,21 +792,21 @@
         <v>10</v>
       </c>
       <c r="B5" s="2">
-        <f>H4 + TIME(0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0.57152777777777763</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5" s="10">
-        <f>B5+TIME(0,C5,0)</f>
+        <f t="shared" si="1"/>
         <v>0.57152777777777763</v>
       </c>
       <c r="E5" s="12">
         <v>12</v>
       </c>
       <c r="F5" s="2">
-        <f>D5+TIME(0,E5,0)</f>
+        <f t="shared" si="2"/>
         <v>0.57986111111111094</v>
       </c>
       <c r="G5" s="6">
@@ -813,21 +828,21 @@
         <v>9</v>
       </c>
       <c r="B6" s="2">
-        <f>H5 + TIME(0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0.58055555555555538</v>
       </c>
       <c r="C6" s="4">
         <v>2</v>
       </c>
       <c r="D6" s="10">
-        <f>B6+TIME(0,C6,0)</f>
+        <f t="shared" si="1"/>
         <v>0.58194444444444426</v>
       </c>
       <c r="E6" s="12">
         <v>30</v>
       </c>
       <c r="F6" s="2">
-        <f>D6+TIME(0,E6,0)</f>
+        <f t="shared" si="2"/>
         <v>0.60277777777777763</v>
       </c>
       <c r="G6" s="6">
@@ -850,21 +865,21 @@
         <v>8</v>
       </c>
       <c r="B7" s="2">
-        <f>H6 + TIME(0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0.59930555555555542</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7" s="10">
-        <f>B7+TIME(0,C7,0)</f>
+        <f t="shared" si="1"/>
         <v>0.59930555555555542</v>
       </c>
       <c r="E7" s="12">
         <v>17</v>
       </c>
       <c r="F7" s="2">
-        <f>D7+TIME(0,E7,0)</f>
+        <f t="shared" si="2"/>
         <v>0.61111111111111094</v>
       </c>
       <c r="G7" s="6">
@@ -887,21 +902,21 @@
         <v>15</v>
       </c>
       <c r="B8" s="2">
-        <f>H7 + TIME(0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0.60763888888888873</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8" s="10">
-        <f>B8+TIME(0,C8,0)</f>
+        <f t="shared" si="1"/>
         <v>0.60763888888888873</v>
       </c>
       <c r="E8" s="12">
         <v>96</v>
       </c>
       <c r="F8" s="2">
-        <f>D8+TIME(0,E8,0)</f>
+        <f t="shared" si="2"/>
         <v>0.67430555555555538</v>
       </c>
       <c r="G8" s="6">
@@ -1109,8 +1124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R117"/>
   <sheetViews>
-    <sheetView topLeftCell="I94" workbookViewId="0">
-      <selection activeCell="L116" sqref="L116"/>
+    <sheetView topLeftCell="F98" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:R117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1166,7 +1181,7 @@
         <v>38</v>
       </c>
       <c r="F2" s="21">
-        <v>43484.539583333331</v>
+        <v>43484.522222222222</v>
       </c>
       <c r="G2" s="14">
         <v>115.867</v>
@@ -1197,12 +1212,12 @@
         <v>154</v>
       </c>
       <c r="O2">
-        <f>N2/9</f>
-        <v>17.111111111111111</v>
+        <f>N2/8</f>
+        <v>19.25</v>
       </c>
       <c r="R2" s="19" t="str">
         <f>CONCATENATE(A2,";",B2,";",C2,";",D2,";",E2,";",TEXT(F2, "gg-mm-aaaa hh:mm:ss"),,";",G2,";",H2,)</f>
-        <v>1;14,66403637;41,55812783;Stazione;temp stazioni xy;19-01-2019 12:57:00;115,867;18,247</v>
+        <v>1;14,66403637;41,55812783;Stazione;temp stazioni xy;19-01-2019 12:32:00;115,867;18,247</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -1221,9 +1236,8 @@
       <c r="E3" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="20">
-        <f>F2+TIME(0,0,(G3/$H$2) + $O$2)</f>
-        <v>43484.539918981478</v>
+      <c r="F3" s="21">
+        <v>43484.539583333331</v>
       </c>
       <c r="G3" s="14">
         <v>219.74600000000001</v>
@@ -1238,7 +1252,7 @@
       </c>
       <c r="R3" s="19" t="str">
         <f t="shared" ref="R3:R66" si="0">CONCATENATE(A3,";",B3,";",C3,";",D3,";",E3,";",TEXT(F3, "gg-mm-aaaa hh:mm:ss"),,";",G3,";",H3,)</f>
-        <v>2;14,66266037;41,5564407;Scalo ferroviario;temp stazioni xy;19-01-2019 12:57:29;219,746;</v>
+        <v>2;14,66266037;41,5564407;Scalo ferroviario;temp stazioni xy;19-01-2019 12:57:00;219,746;</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -1259,14 +1273,14 @@
       </c>
       <c r="F4" s="20">
         <f t="shared" ref="F4:F11" si="1">F3+TIME(0,0,(G4/$H$2) + $O$2)</f>
-        <v>43484.540150462963</v>
+        <v>43484.539837962962</v>
       </c>
       <c r="G4" s="14">
         <v>61.131999999999998</v>
       </c>
       <c r="R4" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>3;14,66240712;41,5559242;Scalo ferroviario;temp stazioni xy;19-01-2019 12:57:49;61,132;</v>
+        <v>3;14,66240712;41,5559242;Scalo ferroviario;temp stazioni xy;19-01-2019 12:57:22;61,132;</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -1287,14 +1301,14 @@
       </c>
       <c r="F5" s="20">
         <f t="shared" si="1"/>
-        <v>43484.540358796294</v>
+        <v>43484.540069444447</v>
       </c>
       <c r="G5" s="14">
         <v>27.573</v>
       </c>
       <c r="R5" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>4;14,66216862;41,55575233;Scalo ferroviario;temp stazioni xy;19-01-2019 12:58:07;27,573;</v>
+        <v>4;14,66216862;41,55575233;Scalo ferroviario;temp stazioni xy;19-01-2019 12:57:42;27,573;</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1313,14 +1327,14 @@
       </c>
       <c r="F6" s="20">
         <f t="shared" si="1"/>
-        <v>43484.542731481481</v>
+        <v>43484.54246527778</v>
       </c>
       <c r="G6" s="14">
         <v>3441.86</v>
       </c>
       <c r="R6" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>5;14,63184412;41,53474358;;temp punti xy;19-01-2019 13:01:32;3441,86;</v>
+        <v>5;14,63184412;41,53474358;;temp punti xy;19-01-2019 13:01:09;3441,86;</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -1339,14 +1353,14 @@
       </c>
       <c r="F7" s="20">
         <f t="shared" si="1"/>
-        <v>43484.544918981483</v>
+        <v>43484.544675925928</v>
       </c>
       <c r="G7" s="14">
         <v>3146.2159999999999</v>
       </c>
       <c r="R7" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>6;14,59737549;41,52327233;;temp punti xy;19-01-2019 13:04:41;3146,216;</v>
+        <v>6;14,59737549;41,52327233;;temp punti xy;19-01-2019 13:04:20;3146,216;</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -1365,14 +1379,14 @@
       </c>
       <c r="F8" s="20">
         <f t="shared" si="1"/>
-        <v>43484.546157407407</v>
+        <v>43484.545937499999</v>
       </c>
       <c r="G8" s="14">
         <v>1644.4159999999999</v>
       </c>
       <c r="R8" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>7;14,58860349;41,5100152;;temp punti xy;19-01-2019 13:06:28;1644,416;</v>
+        <v>7;14,58860349;41,5100152;;temp punti xy;19-01-2019 13:06:09;1644,416;</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1391,14 +1405,14 @@
       </c>
       <c r="F9" s="20">
         <f t="shared" si="1"/>
-        <v>43484.547199074077</v>
+        <v>43484.547013888885</v>
       </c>
       <c r="G9" s="14">
         <v>1346.76</v>
       </c>
       <c r="R9" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>8;14,60397374;41,50633383;;temp punti xy;19-01-2019 13:07:58;1346,76;</v>
+        <v>8;14,60397374;41,50633383;;temp punti xy;19-01-2019 13:07:42;1346,76;</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -1419,14 +1433,14 @@
       </c>
       <c r="F10" s="20">
         <f t="shared" si="1"/>
-        <v>43484.548263888893</v>
+        <v>43484.548101851848</v>
       </c>
       <c r="G10" s="14">
         <v>1381.1379999999999</v>
       </c>
       <c r="R10" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>9;14,59945299;41,4943717;Scalo ferroviario;temp stazioni xy;19-01-2019 13:09:30;1381,138;</v>
+        <v>9;14,59945299;41,4943717;Scalo ferroviario;temp stazioni xy;19-01-2019 13:09:16;1381,138;</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -1447,14 +1461,14 @@
       </c>
       <c r="F11" s="20">
         <f t="shared" si="1"/>
-        <v>43484.548483796301</v>
+        <v>43484.548344907402</v>
       </c>
       <c r="G11" s="14">
         <v>38.271000000000001</v>
       </c>
       <c r="R11" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>10;14,59904249;41,49421845;Scalo ferroviario;temp stazioni xy;19-01-2019 13:09:49;38,271;</v>
+        <v>10;14,59904249;41,49421845;Scalo ferroviario;temp stazioni xy;19-01-2019 13:09:37;38,271;</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -4436,9 +4450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4494,7 +4506,7 @@
         <v>38</v>
       </c>
       <c r="F2" s="18">
-        <v>43484.539583333331</v>
+        <v>43484.522222222222</v>
       </c>
       <c r="G2">
         <v>115.867</v>
@@ -4520,7 +4532,7 @@
         <v>38</v>
       </c>
       <c r="F3" s="18">
-        <v>43484.539918981478</v>
+        <v>43484.539583333331</v>
       </c>
       <c r="G3">
         <v>219.74600000000001</v>
@@ -4543,7 +4555,7 @@
         <v>38</v>
       </c>
       <c r="F4" s="18">
-        <v>43484.540150462963</v>
+        <v>43484.539837962962</v>
       </c>
       <c r="G4">
         <v>61.131999999999998</v>
@@ -4566,7 +4578,7 @@
         <v>38</v>
       </c>
       <c r="F5" s="18">
-        <v>43484.540358796294</v>
+        <v>43484.540069444447</v>
       </c>
       <c r="G5">
         <v>27.573</v>
@@ -4586,7 +4598,7 @@
         <v>39</v>
       </c>
       <c r="F6" s="18">
-        <v>43484.542731481481</v>
+        <v>43484.54246527778</v>
       </c>
       <c r="G6">
         <v>3441.86</v>
@@ -4606,7 +4618,7 @@
         <v>39</v>
       </c>
       <c r="F7" s="18">
-        <v>43484.544918981483</v>
+        <v>43484.544675925928</v>
       </c>
       <c r="G7">
         <v>3146.2159999999999</v>
@@ -4626,7 +4638,7 @@
         <v>39</v>
       </c>
       <c r="F8" s="18">
-        <v>43484.546157407407</v>
+        <v>43484.545937499999</v>
       </c>
       <c r="G8">
         <v>1644.4159999999999</v>
@@ -4646,7 +4658,7 @@
         <v>39</v>
       </c>
       <c r="F9" s="18">
-        <v>43484.547199074077</v>
+        <v>43484.547013888892</v>
       </c>
       <c r="G9">
         <v>1346.76</v>
@@ -4669,7 +4681,7 @@
         <v>38</v>
       </c>
       <c r="F10" s="18">
-        <v>43484.548263888886</v>
+        <v>43484.548101851855</v>
       </c>
       <c r="G10">
         <v>1381.1379999999999</v>
@@ -4692,7 +4704,7 @@
         <v>38</v>
       </c>
       <c r="F11" s="18">
-        <v>43484.548483796294</v>
+        <v>43484.548344907409</v>
       </c>
       <c r="G11">
         <v>38.271000000000001</v>

</xml_diff>